<commit_message>
start over with CMOCK
</commit_message>
<xml_diff>
--- a/test/test_cases.xlsx
+++ b/test/test_cases.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auhn2\Desktop\swift act challenge\speedcontrol\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4949EE7-A8CF-4A6F-8954-3B2683BE92CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D014F4-852A-4475-98D1-1089EC47627B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Combined implementation" sheetId="1" r:id="rId1"/>
+    <sheet name="2 defines" sheetId="2" r:id="rId2"/>
+    <sheet name="2 defines (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="47">
   <si>
     <t>switch state</t>
   </si>
@@ -136,13 +138,43 @@
   </si>
   <si>
     <t>partition_7</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>NEGATIVE_VALUES</t>
+  </si>
+  <si>
+    <t>PB_PRESSURE</t>
+  </si>
+  <si>
+    <t>PB_RELEASED</t>
+  </si>
+  <si>
+    <t>PB_PRE_PRESSED</t>
+  </si>
+  <si>
+    <t>PB_PRESSED</t>
+  </si>
+  <si>
+    <t>PB_PRE_RELEASED</t>
+  </si>
+  <si>
+    <t>PB_MINUS</t>
+  </si>
+  <si>
+    <t>PB_PLUS</t>
+  </si>
+  <si>
+    <t>HIGHER_VALUES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +223,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -218,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -595,11 +640,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -668,118 +750,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,10 +774,288 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1079,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,13 +1354,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="2" spans="1:5" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
@@ -1119,13 +1380,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
@@ -1151,13 +1412,13 @@
       <c r="B5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="52">
         <v>2</v>
       </c>
     </row>
@@ -1168,9 +1429,9 @@
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="45"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="53"/>
     </row>
     <row r="7" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
@@ -1179,13 +1440,13 @@
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="39">
         <v>3</v>
       </c>
     </row>
@@ -1193,41 +1454,41 @@
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="60"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="40"/>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="60"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="61"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="41"/>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="70"/>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
@@ -1236,13 +1497,13 @@
       <c r="B12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="28">
         <v>3</v>
       </c>
     </row>
@@ -1253,13 +1514,13 @@
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="51">
+      <c r="E13" s="32">
         <v>4</v>
       </c>
     </row>
@@ -1270,24 +1531,24 @@
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="52"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="63">
         <v>5</v>
       </c>
     </row>
@@ -1295,28 +1556,28 @@
       <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="31"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="64"/>
     </row>
     <row r="17" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="32"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="65"/>
     </row>
     <row r="18" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="59"/>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
@@ -1325,13 +1586,13 @@
       <c r="B19" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="65" t="s">
+      <c r="D19" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="66">
         <v>5</v>
       </c>
     </row>
@@ -1342,9 +1603,9 @@
       <c r="B20" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="55"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="67"/>
     </row>
     <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1353,13 +1614,13 @@
       <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="51">
+      <c r="E21" s="32">
         <v>6</v>
       </c>
     </row>
@@ -1370,24 +1631,24 @@
       <c r="B22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="52"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="63">
         <v>7</v>
       </c>
     </row>
@@ -1395,36 +1656,22 @@
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="31"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="64"/>
     </row>
     <row r="25" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="32"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="A18:E18"/>
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="E23:E25"/>
     <mergeCell ref="C13:C14"/>
@@ -1436,11 +1683,937 @@
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A11:E11"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E15:E17"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F7433A-CF4C-4229-96A1-B08398F69CA8}">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48"/>
+    </row>
+    <row r="2" spans="1:6" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="74" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="81"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="64"/>
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="82"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="87"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="82"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="90"/>
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="87"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="82"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="90"/>
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="87"/>
+      <c r="B8" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="82"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="90"/>
+    </row>
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="87"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="82"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="90"/>
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="87"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="92" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="82"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="90"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="87"/>
+      <c r="B11" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="93"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="94"/>
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="87"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="96"/>
+      <c r="F12" s="97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="87"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="98"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="100"/>
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A14" s="87"/>
+      <c r="B14" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="91"/>
+      <c r="F14" s="101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="87"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="82"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="102"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="103"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="105" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="82"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="102"/>
+    </row>
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A17" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="82"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="102"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A18" s="87"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="82"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="102"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A19" s="87"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="82"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="102"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="87"/>
+      <c r="B20" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="93"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="107"/>
+    </row>
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A21" s="87"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="108" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="109"/>
+      <c r="F21" s="110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="87"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="92" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="98"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="112"/>
+    </row>
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A23" s="87"/>
+      <c r="B23" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="113" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="114"/>
+      <c r="F23" s="115">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A24" s="87"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="116"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="117"/>
+    </row>
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A25" s="87"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="116"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="117"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A26" s="87"/>
+      <c r="B26" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="116"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="117"/>
+    </row>
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A27" s="87"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="116"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="117"/>
+    </row>
+    <row r="28" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="103"/>
+      <c r="B28" s="104"/>
+      <c r="C28" s="105" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="116"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="117"/>
+    </row>
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A29" s="118" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="118" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="61"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="117"/>
+    </row>
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A30" s="120"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="61"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="117"/>
+    </row>
+    <row r="31" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="120"/>
+      <c r="B31" s="120"/>
+      <c r="C31" s="121" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="122"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="101"/>
+    </row>
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A32" s="120"/>
+      <c r="B32" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="108" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="109"/>
+      <c r="F32" s="110">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="120"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="123" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="98"/>
+      <c r="E33" s="111"/>
+      <c r="F33" s="112"/>
+    </row>
+    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A34" s="120"/>
+      <c r="B34" s="120"/>
+      <c r="C34" s="121" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="124" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="114"/>
+      <c r="F34" s="125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A35" s="120"/>
+      <c r="B35" s="120" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="61"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="102"/>
+    </row>
+    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A36" s="120"/>
+      <c r="B36" s="120"/>
+      <c r="C36" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="61"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="102"/>
+    </row>
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A37" s="120"/>
+      <c r="B37" s="120"/>
+      <c r="C37" s="121" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="61"/>
+      <c r="E37" s="91"/>
+      <c r="F37" s="102"/>
+    </row>
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A38" s="120"/>
+      <c r="B38" s="120" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="61"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="102"/>
+    </row>
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A39" s="120"/>
+      <c r="B39" s="120"/>
+      <c r="C39" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="61"/>
+      <c r="E39" s="91"/>
+      <c r="F39" s="102"/>
+    </row>
+    <row r="40" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="126"/>
+      <c r="B40" s="126"/>
+      <c r="C40" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="61"/>
+      <c r="E40" s="91"/>
+      <c r="F40" s="102"/>
+    </row>
+    <row r="41" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="129"/>
+      <c r="C41" s="130" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="116"/>
+      <c r="E41" s="91"/>
+      <c r="F41" s="115"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="F34:F41"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="D23:D31"/>
+    <mergeCell ref="F23:F31"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A29:A40"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="D34:D41"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="D14:D20"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="A17:A28"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D11"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A5:A16"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="F5:F11"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D418AC09-70CE-474D-BE7F-63E05C206672}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48"/>
+    </row>
+    <row r="2" spans="1:6" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="74" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="65"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="64"/>
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="82"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="87"/>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="82"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="90"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="87"/>
+      <c r="B7" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="131" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="93"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="94"/>
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="87"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="96"/>
+      <c r="F8" s="97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="87"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="98"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="100"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="87"/>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="91"/>
+      <c r="F10" s="101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="82"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="102"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="87"/>
+      <c r="B12" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="131" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="93"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="107"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="87"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="108" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="109"/>
+      <c r="F13" s="110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="87"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="92" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="98"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="112"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="87"/>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="113" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="114"/>
+      <c r="F15" s="115">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="87"/>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="116"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="117"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="118" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="127" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="61"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="117"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A18" s="120"/>
+      <c r="B18" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="123" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="108" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="109"/>
+      <c r="F18" s="110">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="120"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="123" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="98"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="112"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="120"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="92" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="124" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="114"/>
+      <c r="F20" s="125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="120"/>
+      <c r="B21" s="121" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="61"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="102"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="120"/>
+      <c r="B22" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="61"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="102"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="129"/>
+      <c r="C23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="116"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="115"/>
+    </row>
+    <row r="24" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="128" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="B7:B9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>